<commit_message>
Elaboración de gráfica y funciones para el analisis de stock
</commit_message>
<xml_diff>
--- a/Alerta_Reabastecimiento.xlsx
+++ b/Alerta_Reabastecimiento.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,11 +437,6 @@
           <t>stock</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>valor_total_stock</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -455,9 +450,6 @@
       <c r="C2" t="n">
         <v>2</v>
       </c>
-      <c r="D2" t="n">
-        <v>400</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -471,9 +463,6 @@
       <c r="C3" t="n">
         <v>2</v>
       </c>
-      <c r="D3" t="n">
-        <v>800</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>